<commit_message>
solved for the case (11920)where 1920 was detected as a year
</commit_message>
<xml_diff>
--- a/PublicationsExcel2021b.xlsx
+++ b/PublicationsExcel2021b.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25180" windowHeight="10720" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25180" windowHeight="11860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AEK-Publications" sheetId="1" r:id="rId1"/>
     <sheet name="Presentations" sheetId="2" r:id="rId2"/>
     <sheet name="Reports" sheetId="3" r:id="rId3"/>
-    <sheet name="YearColumnReports" sheetId="4" r:id="rId4"/>
+    <sheet name="year_column_added" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="378">
   <si>
     <t>No</t>
   </si>
@@ -1080,6 +1080,9 @@
     <t>Büyükhatipoglu S., L. Bat, A. Kideys, S. Tugrul, J. Zagorodnyaya, A. Gundogdu, M. Akbulut, M. Culha, G. Gonlugor, E. Eker &amp; H. H. Satilmis 2002. Orta Karadeniz’in Sinop Burnu bölgesinin biyokimyasal dönüşüm çalışmaları. TÜBİTAK YDABÇAG 619/G 197Y156 Projesi Final Raporu, Mart 2002, 92 s.</t>
   </si>
   <si>
+    <t>TUBITAK TOZ ara raporları…2004</t>
+  </si>
+  <si>
     <t>NATO Ara raporları…2002?</t>
   </si>
   <si>
@@ -1095,64 +1098,64 @@
     <t>Rapana raporlari…2006?</t>
   </si>
   <si>
+    <t>TUBITAK11923 Calanus 2004?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kideys, A. E., Kourti, N., Shepherd, I., Greidanus, H., Thoorens, F-X., Cesena, C., Sahin, F., Ozdemir, S., Satilmis, H.H., Bat, L. (2006). Behaviour, effort characteristics, catch and remote sensing detection of Turkish fishing vessels during anchovy fishery in the Black Sea in 2005-2006. Final Report to the European Commission for the Joint Research Center (JRC), Tender Proposal No G03/07/05, 43 pages, April, 2006. </t>
+  </si>
+  <si>
+    <t>Kideys A. E., T. Barbas, E. Varol, F. Sahin, H. Greidanus, L. Bat, E. Duzgunes, A. Guneroglu, I. Okumus, F. Kalayci, G. Dalgic, N. Samsun, H. H. Satilmis, S. Ozdemir (2007). Feasibility of monitoring fishing vessel activity in the Black Sea using automatic identification system (AIS) technology. Final Report, 93 pages, Joint Research Center, Ispra, Italy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Özhan K. A.E. Kıdeyş, B. Salihoğlu, O. Güven, V. Myroshnychenko, A. C. Gücü, S. Tuğrul 2016. Mersin Körfezi oşinografik/kirlilik izleme projesi. Final Raporu, 70 s. Destekleyen Kurum: Mersin Büyükşehir Belediyesi), Yürütücü Kurum: ODTÜ Deniz Bilimleri Enstitüsü.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kıdeyş A.E., K. Özkan, B. Salihoğlu, V. Myroshnychenko 2017. Mersin kıyılarında deniz kaplumbağalarının ve iklim değişikliğinin deniz kaplumbağaları üzerindeki etkilerinin izlenmesi ile denizlerin korunması konusunda orta öğretim çocuklarında farkındalık yaratma projesi. Final Raporu, 48 s. Destekleyen Kurum: Mersin Büyükşehir Belediyesi), Yürütücü Kurum: ODTÜ Deniz Bilimleri Enstitüsü. </t>
+  </si>
+  <si>
+    <t>Kideys et al. 2012? ve sonraki yıllar. ”I know and protect my sea”: Applied Marine Science Education directed at the primary school children. Sponsored by TUBITAK during 2012-2015 and by Mersin Greater City Municipality during 2016 and 2017. First and last two years coordinator, other years participant.</t>
+  </si>
+  <si>
+    <t>ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Akdeniz Özet Raporu, ISBN:978-605-5294-68-7, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 61 sy., ANKARA-2017. </t>
+  </si>
+  <si>
+    <t>Elitsa Stefanova, Violeta Slabakova, Kremena Stefanova, Volodymyr Myroshnychenko, Ahmet Kideys, Tamara Shiganova. Appropriateness and availability of the Mnemiopsis leidyi and Beroe ovata data on the Black sea. In: 14th International conference on marine sciences and technologies Black Sea 2018. Proceedings, ISSN 1314-0957, October 2018, Varna, Bulgaria, pp.245-250. DOI: https://doi.org/10.7546/IO.BAS.2018.3</t>
+  </si>
+  <si>
+    <t>2.Polat-Beken Ç., L. Tolun, H. Atabay, I. Tan, M. Mantıkcı, C. Aydöner, D. Ediger, A. Yüksek, H. Altıok, S. Taş, Y. Gürkan, M. Sezgı̇n, G. Kurt Şahin, F. Ünlüer, E. Taşkın, O. Minareci, M. Çakır, A. E. Kıdeys, S. Tuğrul 2017a. Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Marmara Denizi Özet Raporu. ÇŞB-ÇEDİDGM, TÜBİTAK-MAM, ISBN:978-605-5294-72-4, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 71 sy., ANKARA-2017. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polat-Beken Ç., H. Atabay, M. Mantıkcı, I. Tan, L. Tolun, S. Mutlu, E. Aslan, , M. Sezgı̇n,F. Şahin, G. Kurt Şahin, F. Ünlüer, E. Taşkın, O. Minareci, M. Çakır,S. Karakulak, A.E. Kahraman, B. Gül, F.Telli Karakoç, E. Düzgüneş, C. Erüz and  A. E. Kıdeys 2017b. Deni̇zlerde Bütünleşi̇k Ki̇rli̇li̇k İzleme Programi 2014-2016 Karadeni̇z Özet Raporu. TÜBİTAK MAM Matbaası Gebze/Kocaeli 5148704 (ÇTÜE.16.329). </t>
+  </si>
+  <si>
+    <t>ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Ege Denizi Özet Raporu, ISBN:978-605-5294-69-4, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 68 sy., ANKARA-2017. </t>
+  </si>
+  <si>
+    <t>4.      ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Karadeniz Özet Raporu, ISBN:978-605-5294-70-0, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 69 sy., ANKARA-2017.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kideys A.E., B. Halisdemir, A. Kideys , A. C. Gucu, A. Gazihan, B. Salihoglu, B. Yapan, B. Temiz, G. Akkus, K. Gokdag, K. Ozkan, M. Ok, M. Kurt, M. Yucel, O. Karakus, G. Can 2018. A University – Municipality partnership: Marine Environmental Awareness training (k12) in Turkey. Abstract published in the EMSEA (European Marine Science Educators Association) Conference Book, 2-5 October 2018, Newcastle-Upon-Tyne, UK, pp 3. (https://conferences.ncl.ac.uk/emsea2018/) </t>
+  </si>
+  <si>
+    <t>Kideys A.E., K. Gökdağ, O. Güven, B. Jovanovic, Y. Emre, D. Eraslan &amp; B. Salihoğlu 2018. Estimating the quantity and composition of microplastics in the Mediterranean coast of Turkey; the potential for bioaccumulation in seafood (Türkiye’nin Akdeniz Sahillerinde Mikro-Plastik Kompozisyonu ve Miktarının Belirlenmesi; Mikro- Plastiklerin Deniz Ürünlerinde Olası Biyolojik Birikimi). TÜBİTAK 145Y244 nolu 1001 Projesi Final Raporu. ODTÜ Deniz Bilimleri Enstitüsü, 92s.</t>
+  </si>
+  <si>
+    <t>Kideys A.E., Y. Ak-Örek, M. Yılmaz, K. Özhan, A. Karahan, B. Salihoğlu, K. Gökdağ, E. Kocaman 2018. Mikroplastik Partiküllerin ve Plastik Katkısı Olan "Bisfenol A" Organik Bileşiğinin Mersin Körfezi'nde Dağılım Gösteren Bazı Zooplankton Türleri Üzerine Etkilerinin Belirlenmesi. TÜBİTAK 115Y627 nolu 1001 Projesi Final Raporu. ODTÜ Deniz Bilimleri Enstitüsü, 129s.</t>
+  </si>
+  <si>
+    <t>Kideys 2018. Mikroplastik1. 2015-2018 Estimating the quantity and composition of microplastics in the Mediterranean coast of Turkey; the potential for bioaccumulation in seafood. Sponsored by TUBITAK. Coordinator.</t>
+  </si>
+  <si>
+    <t>Kideys 2018. Mikroplastik2. 2016-2018 Impacts of microplastic particles and bisphenol A as a chemical additive in zooplankton species of Mersin Bay. Sponsored by TUBITAK. Coordinator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veiga, J., Aydin, M. Koren, S., Kideys, A., Trdan, S. (2019). Marine Litter Indicators – Scoping Study. ETC/ICM Deliverable 6.1.iii. </t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
     <t>TUBITAK Calanus 2004?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kideys, A. E., Kourti, N., Shepherd, I., Greidanus, H., Thoorens, F-X., Cesena, C., Sahin, F., Ozdemir, S., Satilmis, H.H., Bat, L. (2006). Behaviour, effort characteristics, catch and remote sensing detection of Turkish fishing vessels during anchovy fishery in the Black Sea in 2005-2006. Final Report to the European Commission for the Joint Research Center (JRC), Tender Proposal No G03/07/05, 43 pages, April, 2006. </t>
-  </si>
-  <si>
-    <t>Kideys A. E., T. Barbas, E. Varol, F. Sahin, H. Greidanus, L. Bat, E. Duzgunes, A. Guneroglu, I. Okumus, F. Kalayci, G. Dalgic, N. Samsun, H. H. Satilmis, S. Ozdemir (2007). Feasibility of monitoring fishing vessel activity in the Black Sea using automatic identification system (AIS) technology. Final Report, 93 pages, Joint Research Center, Ispra, Italy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Özhan K. A.E. Kıdeyş, B. Salihoğlu, O. Güven, V. Myroshnychenko, A. C. Gücü, S. Tuğrul 2016. Mersin Körfezi oşinografik/kirlilik izleme projesi. Final Raporu, 70 s. Destekleyen Kurum: Mersin Büyükşehir Belediyesi), Yürütücü Kurum: ODTÜ Deniz Bilimleri Enstitüsü.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kıdeyş A.E., K. Özkan, B. Salihoğlu, V. Myroshnychenko 2017. Mersin kıyılarında deniz kaplumbağalarının ve iklim değişikliğinin deniz kaplumbağaları üzerindeki etkilerinin izlenmesi ile denizlerin korunması konusunda orta öğretim çocuklarında farkındalık yaratma projesi. Final Raporu, 48 s. Destekleyen Kurum: Mersin Büyükşehir Belediyesi), Yürütücü Kurum: ODTÜ Deniz Bilimleri Enstitüsü. </t>
-  </si>
-  <si>
-    <t>Kideys et al. 2012? ve sonraki yıllar. ”I know and protect my sea”: Applied Marine Science Education directed at the primary school children. Sponsored by TUBITAK during 2012-2015 and by Mersin Greater City Municipality during 2016 and 2017. First and last two years coordinator, other years participant.</t>
-  </si>
-  <si>
-    <t>ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Akdeniz Özet Raporu, ISBN:978-605-5294-68-7, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 61 sy., ANKARA-2017. </t>
-  </si>
-  <si>
-    <t>Elitsa Stefanova, Violeta Slabakova, Kremena Stefanova, Volodymyr Myroshnychenko, Ahmet Kideys, Tamara Shiganova. Appropriateness and availability of the Mnemiopsis leidyi and Beroe ovata data on the Black sea. In: 14th International conference on marine sciences and technologies Black Sea 2018. Proceedings, ISSN 1314-0957, October 2018, Varna, Bulgaria, pp.245-250. DOI: https://doi.org/10.7546/IO.BAS.2018.3</t>
-  </si>
-  <si>
-    <t>2.Polat-Beken Ç., L. Tolun, H. Atabay, I. Tan, M. Mantıkcı, C. Aydöner, D. Ediger, A. Yüksek, H. Altıok, S. Taş, Y. Gürkan, M. Sezgı̇n, G. Kurt Şahin, F. Ünlüer, E. Taşkın, O. Minareci, M. Çakır, A. E. Kıdeys, S. Tuğrul 2017a. Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Marmara Denizi Özet Raporu. ÇŞB-ÇEDİDGM, TÜBİTAK-MAM, ISBN:978-605-5294-72-4, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 71 sy., ANKARA-2017. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polat-Beken Ç., H. Atabay, M. Mantıkcı, I. Tan, L. Tolun, S. Mutlu, E. Aslan, , M. Sezgı̇n,F. Şahin, G. Kurt Şahin, F. Ünlüer, E. Taşkın, O. Minareci, M. Çakır,S. Karakulak, A.E. Kahraman, B. Gül, F.Telli Karakoç, E. Düzgüneş, C. Erüz and  A. E. Kıdeys 2017b. Deni̇zlerde Bütünleşi̇k Ki̇rli̇li̇k İzleme Programi 2014-2016 Karadeni̇z Özet Raporu. TÜBİTAK MAM Matbaası Gebze/Kocaeli 5148704 (ÇTÜE.16.329). </t>
-  </si>
-  <si>
-    <t>ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Ege Denizi Özet Raporu, ISBN:978-605-5294-69-4, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 68 sy., ANKARA-2017. </t>
-  </si>
-  <si>
-    <t>4.      ÇŞB-ÇEDİDGM, TÜBİTAK-MAM (2017) Denizlerde Bütünleşik Kirlilik İzleme İşi 2014-2016 Karadeniz Özet Raporu, ISBN:978-605-5294-70-0, TÜBİTAK MAM Matbaası Gebze/Kocaeli, 69 sy., ANKARA-2017.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kideys A.E., B. Halisdemir, A. Kideys , A. C. Gucu, A. Gazihan, B. Salihoglu, B. Yapan, B. Temiz, G. Akkus, K. Gokdag, K. Ozkan, M. Ok, M. Kurt, M. Yucel, O. Karakus, G. Can 2018. A University – Municipality partnership: Marine Environmental Awareness training (k12) in Turkey. Abstract published in the EMSEA (European Marine Science Educators Association) Conference Book, 2-5 October 2018, Newcastle-Upon-Tyne, UK, pp 3. (https://conferences.ncl.ac.uk/emsea2018/) </t>
-  </si>
-  <si>
-    <t>Kideys A.E., K. Gökdağ, O. Güven, B. Jovanovic, Y. Emre, D. Eraslan &amp; B. Salihoğlu 2018. Estimating the quantity and composition of microplastics in the Mediterranean coast of Turkey; the potential for bioaccumulation in seafood (Türkiye’nin Akdeniz Sahillerinde Mikro-Plastik Kompozisyonu ve Miktarının Belirlenmesi; Mikro- Plastiklerin Deniz Ürünlerinde Olası Biyolojik Birikimi). TÜBİTAK 145Y244 nolu 1001 Projesi Final Raporu. ODTÜ Deniz Bilimleri Enstitüsü, 92s.</t>
-  </si>
-  <si>
-    <t>Kideys A.E., Y. Ak-Örek, M. Yılmaz, K. Özhan, A. Karahan, B. Salihoğlu, K. Gökdağ, E. Kocaman 2018. Mikroplastik Partiküllerin ve Plastik Katkısı Olan "Bisfenol A" Organik Bileşiğinin Mersin Körfezi'nde Dağılım Gösteren Bazı Zooplankton Türleri Üzerine Etkilerinin Belirlenmesi. TÜBİTAK 115Y627 nolu 1001 Projesi Final Raporu. ODTÜ Deniz Bilimleri Enstitüsü, 129s.</t>
-  </si>
-  <si>
-    <t>Kideys 2018. Mikroplastik1. 2015-2018 Estimating the quantity and composition of microplastics in the Mediterranean coast of Turkey; the potential for bioaccumulation in seafood. Sponsored by TUBITAK. Coordinator.</t>
-  </si>
-  <si>
-    <t>Kideys 2018. Mikroplastik2. 2016-2018 Impacts of microplastic particles and bisphenol A as a chemical additive in zooplankton species of Mersin Bay. Sponsored by TUBITAK. Coordinator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veiga, J., Aydin, M. Koren, S., Kideys, A., Trdan, S. (2019). Marine Litter Indicators – Scoping Study. ETC/ICM Deliverable 6.1.iii. </t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>TUBITAK TOZ ara raporları…2004</t>
   </si>
 </sst>
 </file>
@@ -1882,7 +1885,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1893,10 +1896,10 @@
   <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4039,7 +4042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A124"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -4677,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4878,122 +4883,122 @@
     </row>
     <row r="39" spans="1:1" ht="15.75" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.75" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.75" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.75" customHeight="1">
       <c r="A43" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" customHeight="1">
       <c r="A44" s="23" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" customHeight="1">
       <c r="A45" s="23" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" customHeight="1">
       <c r="A46" s="23" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15.75" customHeight="1">
       <c r="A47" s="23" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15.75" customHeight="1">
       <c r="A48" s="23" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15.75" customHeight="1">
       <c r="A49" s="23" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15.75" customHeight="1">
       <c r="A50" s="32" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="29" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="25" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="27" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" customHeight="1">
       <c r="A54" s="28" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="29" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="26" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="30" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15.75" customHeight="1">
       <c r="A60" s="24" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15.75" customHeight="1">
       <c r="A61" s="24" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" customHeight="1">
       <c r="A62" s="23" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -5013,13 +5018,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0"/>
+    <sheetView topLeftCell="A43" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="34" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>3</v>
@@ -5437,7 +5442,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="C39" t="s">
         <v>101</v>
@@ -5448,7 +5453,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
@@ -5459,7 +5464,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C41" t="s">
         <v>130</v>
@@ -5470,7 +5475,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C42" t="s">
         <v>108</v>
@@ -5481,7 +5486,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C43" t="s">
         <v>101</v>
@@ -5492,7 +5497,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C44" t="s">
         <v>81</v>
@@ -5503,7 +5508,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C45" t="s">
         <v>101</v>
@@ -5514,7 +5519,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C46" t="s">
         <v>81</v>
@@ -5525,7 +5530,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C47" t="s">
         <v>76</v>
@@ -5536,7 +5541,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
@@ -5547,7 +5552,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C49" t="s">
         <v>36</v>
@@ -5558,7 +5563,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C50" t="s">
         <v>54</v>
@@ -5569,7 +5574,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C51" t="s">
         <v>36</v>
@@ -5580,7 +5585,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C52" t="s">
         <v>32</v>
@@ -5591,7 +5596,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C53" t="s">
         <v>36</v>
@@ -5602,7 +5607,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C54" t="s">
         <v>36</v>
@@ -5613,7 +5618,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C55" t="s">
         <v>36</v>
@@ -5624,7 +5629,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C56" t="s">
         <v>36</v>
@@ -5635,7 +5640,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
@@ -5646,7 +5651,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C58" t="s">
         <v>32</v>
@@ -5657,7 +5662,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C59" t="s">
         <v>32</v>
@@ -5668,7 +5673,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C60" t="s">
         <v>32</v>
@@ -5679,7 +5684,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C61" t="s">
         <v>32</v>
@@ -5690,7 +5695,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>

</xml_diff>